<commit_message>
Daily attendance processing - 2025-08-31 03:39:39
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
+++ b/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
@@ -637,10 +637,10 @@
         <v>42</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K2" s="5" t="n">
         <v>55</v>
@@ -707,10 +707,10 @@
         <v>42</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>55</v>
@@ -777,10 +777,10 @@
         <v>42</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>55</v>
@@ -847,10 +847,10 @@
         <v>42</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>55</v>
@@ -917,10 +917,10 @@
         <v>42</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>55</v>
@@ -987,10 +987,10 @@
         <v>42</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>55</v>
@@ -1057,10 +1057,10 @@
         <v>42</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>55</v>
@@ -1127,10 +1127,10 @@
         <v>42</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>55</v>
@@ -1197,10 +1197,10 @@
         <v>42</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>55</v>
@@ -1267,10 +1267,10 @@
         <v>42</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>55</v>
@@ -1337,10 +1337,10 @@
         <v>42</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>55</v>
@@ -1407,10 +1407,10 @@
         <v>42</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>55</v>
@@ -1477,10 +1477,10 @@
         <v>42</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>55</v>
@@ -1547,10 +1547,10 @@
         <v>42</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>55</v>
@@ -1617,10 +1617,10 @@
         <v>42</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="5" t="n">
         <v>55</v>
@@ -1687,10 +1687,10 @@
         <v>42</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>55</v>
@@ -1757,10 +1757,10 @@
         <v>42</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>55</v>
@@ -1827,10 +1827,10 @@
         <v>42</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>55</v>
@@ -1897,10 +1897,10 @@
         <v>42</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>55</v>
@@ -1967,10 +1967,10 @@
         <v>42</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>55</v>
@@ -2037,10 +2037,10 @@
         <v>42</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>55</v>
@@ -2107,10 +2107,10 @@
         <v>42</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J23" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>55</v>
@@ -2177,10 +2177,10 @@
         <v>42</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J24" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>55</v>
@@ -2247,10 +2247,10 @@
         <v>42</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J25" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>55</v>
@@ -2317,10 +2317,10 @@
         <v>42</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>55</v>
@@ -2387,10 +2387,10 @@
         <v>42</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J27" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>55</v>
@@ -2457,10 +2457,10 @@
         <v>42</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="5" t="n">
         <v>55</v>
@@ -2527,10 +2527,10 @@
         <v>42</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J29" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>55</v>
@@ -2597,10 +2597,10 @@
         <v>42</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J30" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>55</v>
@@ -2667,10 +2667,10 @@
         <v>42</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J31" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>55</v>
@@ -2737,10 +2737,10 @@
         <v>42</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J32" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>55</v>
@@ -2807,10 +2807,10 @@
         <v>42</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J33" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>55</v>
@@ -2877,10 +2877,10 @@
         <v>42</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J34" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K34" s="5" t="n">
         <v>55</v>
@@ -2947,10 +2947,10 @@
         <v>42</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="5" t="n">
         <v>55</v>
@@ -3017,10 +3017,10 @@
         <v>42</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J36" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K36" s="5" t="n">
         <v>55</v>
@@ -3087,10 +3087,10 @@
         <v>42</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J37" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>55</v>
@@ -3157,10 +3157,10 @@
         <v>42</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J38" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" s="5" t="n">
         <v>55</v>
@@ -3227,10 +3227,10 @@
         <v>42</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J39" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K39" s="5" t="n">
         <v>55</v>
@@ -3297,10 +3297,10 @@
         <v>42</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>55</v>
@@ -3367,10 +3367,10 @@
         <v>42</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J41" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K41" s="5" t="n">
         <v>55</v>
@@ -3437,10 +3437,10 @@
         <v>42</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K42" s="5" t="n">
         <v>55</v>
@@ -3507,10 +3507,10 @@
         <v>42</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J43" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" s="5" t="n">
         <v>55</v>
@@ -3577,10 +3577,10 @@
         <v>42</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J44" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K44" s="5" t="n">
         <v>55</v>
@@ -3647,10 +3647,10 @@
         <v>42</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K45" s="5" t="n">
         <v>55</v>
@@ -3717,10 +3717,10 @@
         <v>42</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46" s="5" t="n">
         <v>55</v>
@@ -3787,10 +3787,10 @@
         <v>42</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" s="5" t="n">
         <v>55</v>
@@ -3857,10 +3857,10 @@
         <v>42</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" s="5" t="n">
         <v>55</v>
@@ -3927,10 +3927,10 @@
         <v>42</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="5" t="n">
         <v>55</v>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-01 03:53:59
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
+++ b/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
@@ -637,10 +637,10 @@
         <v>42</v>
       </c>
       <c r="I2" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K2" s="5" t="n">
         <v>55</v>
@@ -707,10 +707,10 @@
         <v>42</v>
       </c>
       <c r="I3" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K3" s="5" t="n">
         <v>55</v>
@@ -777,10 +777,10 @@
         <v>42</v>
       </c>
       <c r="I4" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J4" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K4" s="5" t="n">
         <v>55</v>
@@ -847,10 +847,10 @@
         <v>42</v>
       </c>
       <c r="I5" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K5" s="5" t="n">
         <v>55</v>
@@ -917,10 +917,10 @@
         <v>42</v>
       </c>
       <c r="I6" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K6" s="5" t="n">
         <v>55</v>
@@ -987,10 +987,10 @@
         <v>42</v>
       </c>
       <c r="I7" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K7" s="5" t="n">
         <v>55</v>
@@ -1057,10 +1057,10 @@
         <v>42</v>
       </c>
       <c r="I8" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K8" s="5" t="n">
         <v>55</v>
@@ -1127,10 +1127,10 @@
         <v>42</v>
       </c>
       <c r="I9" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="5" t="n">
         <v>55</v>
@@ -1197,10 +1197,10 @@
         <v>42</v>
       </c>
       <c r="I10" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K10" s="5" t="n">
         <v>55</v>
@@ -1267,10 +1267,10 @@
         <v>42</v>
       </c>
       <c r="I11" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K11" s="5" t="n">
         <v>55</v>
@@ -1337,10 +1337,10 @@
         <v>42</v>
       </c>
       <c r="I12" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K12" s="5" t="n">
         <v>55</v>
@@ -1407,10 +1407,10 @@
         <v>42</v>
       </c>
       <c r="I13" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" s="5" t="n">
         <v>55</v>
@@ -1477,10 +1477,10 @@
         <v>42</v>
       </c>
       <c r="I14" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J14" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K14" s="5" t="n">
         <v>55</v>
@@ -1547,10 +1547,10 @@
         <v>42</v>
       </c>
       <c r="I15" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J15" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K15" s="5" t="n">
         <v>55</v>
@@ -1617,10 +1617,10 @@
         <v>42</v>
       </c>
       <c r="I16" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J16" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K16" s="5" t="n">
         <v>55</v>
@@ -1687,10 +1687,10 @@
         <v>42</v>
       </c>
       <c r="I17" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J17" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K17" s="5" t="n">
         <v>55</v>
@@ -1757,10 +1757,10 @@
         <v>42</v>
       </c>
       <c r="I18" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K18" s="5" t="n">
         <v>55</v>
@@ -1827,10 +1827,10 @@
         <v>42</v>
       </c>
       <c r="I19" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K19" s="5" t="n">
         <v>55</v>
@@ -1897,10 +1897,10 @@
         <v>42</v>
       </c>
       <c r="I20" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K20" s="5" t="n">
         <v>55</v>
@@ -1967,10 +1967,10 @@
         <v>42</v>
       </c>
       <c r="I21" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K21" s="5" t="n">
         <v>55</v>
@@ -2037,10 +2037,10 @@
         <v>42</v>
       </c>
       <c r="I22" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J22" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K22" s="5" t="n">
         <v>55</v>
@@ -2107,10 +2107,10 @@
         <v>42</v>
       </c>
       <c r="I23" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K23" s="5" t="n">
         <v>55</v>
@@ -2177,10 +2177,10 @@
         <v>42</v>
       </c>
       <c r="I24" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K24" s="5" t="n">
         <v>55</v>
@@ -2247,10 +2247,10 @@
         <v>42</v>
       </c>
       <c r="I25" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K25" s="5" t="n">
         <v>55</v>
@@ -2317,10 +2317,10 @@
         <v>42</v>
       </c>
       <c r="I26" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J26" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K26" s="5" t="n">
         <v>55</v>
@@ -2387,10 +2387,10 @@
         <v>42</v>
       </c>
       <c r="I27" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J27" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K27" s="5" t="n">
         <v>55</v>
@@ -2457,10 +2457,10 @@
         <v>42</v>
       </c>
       <c r="I28" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J28" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K28" s="5" t="n">
         <v>55</v>
@@ -2527,10 +2527,10 @@
         <v>42</v>
       </c>
       <c r="I29" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J29" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K29" s="5" t="n">
         <v>55</v>
@@ -2597,10 +2597,10 @@
         <v>42</v>
       </c>
       <c r="I30" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J30" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K30" s="5" t="n">
         <v>55</v>
@@ -2667,10 +2667,10 @@
         <v>42</v>
       </c>
       <c r="I31" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J31" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K31" s="5" t="n">
         <v>55</v>
@@ -2737,10 +2737,10 @@
         <v>42</v>
       </c>
       <c r="I32" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K32" s="5" t="n">
         <v>55</v>
@@ -2807,10 +2807,10 @@
         <v>42</v>
       </c>
       <c r="I33" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J33" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K33" s="5" t="n">
         <v>55</v>
@@ -2877,10 +2877,10 @@
         <v>42</v>
       </c>
       <c r="I34" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J34" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K34" s="5" t="n">
         <v>55</v>
@@ -2947,10 +2947,10 @@
         <v>42</v>
       </c>
       <c r="I35" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J35" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K35" s="5" t="n">
         <v>55</v>
@@ -3017,10 +3017,10 @@
         <v>42</v>
       </c>
       <c r="I36" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K36" s="5" t="n">
         <v>55</v>
@@ -3087,10 +3087,10 @@
         <v>42</v>
       </c>
       <c r="I37" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K37" s="5" t="n">
         <v>55</v>
@@ -3157,10 +3157,10 @@
         <v>42</v>
       </c>
       <c r="I38" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K38" s="5" t="n">
         <v>55</v>
@@ -3227,10 +3227,10 @@
         <v>42</v>
       </c>
       <c r="I39" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J39" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K39" s="5" t="n">
         <v>55</v>
@@ -3297,10 +3297,10 @@
         <v>42</v>
       </c>
       <c r="I40" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K40" s="5" t="n">
         <v>55</v>
@@ -3367,10 +3367,10 @@
         <v>42</v>
       </c>
       <c r="I41" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K41" s="5" t="n">
         <v>55</v>
@@ -3437,10 +3437,10 @@
         <v>42</v>
       </c>
       <c r="I42" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J42" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K42" s="5" t="n">
         <v>55</v>
@@ -3507,10 +3507,10 @@
         <v>42</v>
       </c>
       <c r="I43" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J43" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K43" s="5" t="n">
         <v>55</v>
@@ -3577,10 +3577,10 @@
         <v>42</v>
       </c>
       <c r="I44" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J44" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K44" s="5" t="n">
         <v>55</v>
@@ -3647,10 +3647,10 @@
         <v>42</v>
       </c>
       <c r="I45" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K45" s="5" t="n">
         <v>55</v>
@@ -3717,10 +3717,10 @@
         <v>42</v>
       </c>
       <c r="I46" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K46" s="5" t="n">
         <v>55</v>
@@ -3787,10 +3787,10 @@
         <v>42</v>
       </c>
       <c r="I47" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K47" s="5" t="n">
         <v>55</v>
@@ -3857,10 +3857,10 @@
         <v>42</v>
       </c>
       <c r="I48" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J48" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K48" s="5" t="n">
         <v>55</v>
@@ -3927,10 +3927,10 @@
         <v>42</v>
       </c>
       <c r="I49" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J49" s="5" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K49" s="5" t="n">
         <v>55</v>

</xml_diff>

<commit_message>
Daily attendance processing - 2025-09-07 03:36:03
</commit_message>
<xml_diff>
--- a/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
+++ b/attendance_reports/Y5_B2425_Pediatrics_attendance.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Attendance" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Summary_updated" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Attendance_updated" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Transfers_updated" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary'!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance'!$A$1:$J$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Summary_updated'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Attendance_updated'!$A$1:$K$115</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Transfers_updated'!$A$1:$F$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -3845,7 +3847,7 @@
         <v>1</v>
       </c>
       <c r="P52" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53">
@@ -3909,7 +3911,7 @@
         <v>1</v>
       </c>
       <c r="P53" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54">
@@ -3973,7 +3975,7 @@
         <v>1</v>
       </c>
       <c r="P54" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
@@ -4037,7 +4039,7 @@
         <v>1</v>
       </c>
       <c r="P55" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
@@ -4101,7 +4103,7 @@
         <v>1</v>
       </c>
       <c r="P56" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
@@ -4165,7 +4167,7 @@
         <v>1</v>
       </c>
       <c r="P57" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -4229,7 +4231,7 @@
         <v>1</v>
       </c>
       <c r="P58" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
@@ -4293,7 +4295,7 @@
         <v>1</v>
       </c>
       <c r="P59" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="60">
@@ -4357,7 +4359,7 @@
         <v>1</v>
       </c>
       <c r="P60" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -4421,7 +4423,7 @@
         <v>1</v>
       </c>
       <c r="P61" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="62">
@@ -4485,7 +4487,7 @@
         <v>1</v>
       </c>
       <c r="P62" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -4549,7 +4551,7 @@
         <v>1</v>
       </c>
       <c r="P63" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64">
@@ -4613,7 +4615,7 @@
         <v>1</v>
       </c>
       <c r="P64" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="65">
@@ -4677,7 +4679,7 @@
         <v>1</v>
       </c>
       <c r="P65" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="66">
@@ -4741,7 +4743,7 @@
         <v>1</v>
       </c>
       <c r="P66" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -4805,7 +4807,7 @@
         <v>1</v>
       </c>
       <c r="P67" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68">
@@ -4869,7 +4871,7 @@
         <v>1</v>
       </c>
       <c r="P68" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
@@ -4933,7 +4935,7 @@
         <v>1</v>
       </c>
       <c r="P69" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
@@ -4997,7 +4999,7 @@
         <v>1</v>
       </c>
       <c r="P70" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
@@ -5061,7 +5063,7 @@
         <v>1</v>
       </c>
       <c r="P71" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -5125,7 +5127,7 @@
         <v>1</v>
       </c>
       <c r="P72" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
@@ -5189,7 +5191,7 @@
         <v>1</v>
       </c>
       <c r="P73" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
@@ -5253,7 +5255,7 @@
         <v>1</v>
       </c>
       <c r="P74" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -6853,7 +6855,7 @@
         <v>1</v>
       </c>
       <c r="P99" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -6917,7 +6919,7 @@
         <v>1</v>
       </c>
       <c r="P100" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
@@ -6981,7 +6983,7 @@
         <v>1</v>
       </c>
       <c r="P101" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
@@ -7045,7 +7047,7 @@
         <v>1</v>
       </c>
       <c r="P102" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103">
@@ -7109,7 +7111,7 @@
         <v>1</v>
       </c>
       <c r="P103" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
@@ -7173,7 +7175,7 @@
         <v>1</v>
       </c>
       <c r="P104" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
@@ -7237,7 +7239,7 @@
         <v>1</v>
       </c>
       <c r="P105" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
@@ -7301,7 +7303,7 @@
         <v>1</v>
       </c>
       <c r="P106" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
@@ -7365,7 +7367,7 @@
         <v>1</v>
       </c>
       <c r="P107" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -7429,7 +7431,7 @@
         <v>1</v>
       </c>
       <c r="P108" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109">
@@ -7493,7 +7495,7 @@
         <v>1</v>
       </c>
       <c r="P109" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
@@ -7557,7 +7559,7 @@
         <v>1</v>
       </c>
       <c r="P110" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
@@ -7621,7 +7623,7 @@
         <v>1</v>
       </c>
       <c r="P111" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -7685,7 +7687,7 @@
         <v>1</v>
       </c>
       <c r="P112" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
@@ -7749,7 +7751,7 @@
         <v>1</v>
       </c>
       <c r="P113" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="114">
@@ -7813,7 +7815,7 @@
         <v>1</v>
       </c>
       <c r="P114" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
@@ -7877,7 +7879,7 @@
         <v>1</v>
       </c>
       <c r="P115" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
@@ -7941,7 +7943,7 @@
         <v>1</v>
       </c>
       <c r="P116" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117">
@@ -8005,7 +8007,7 @@
         <v>1</v>
       </c>
       <c r="P117" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="118">
@@ -8069,7 +8071,7 @@
         <v>1</v>
       </c>
       <c r="P118" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
@@ -8133,7 +8135,7 @@
         <v>1</v>
       </c>
       <c r="P119" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120">
@@ -8197,7 +8199,7 @@
         <v>1</v>
       </c>
       <c r="P120" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
@@ -8261,7 +8263,7 @@
         <v>1</v>
       </c>
       <c r="P121" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
@@ -8325,7 +8327,7 @@
         <v>1</v>
       </c>
       <c r="P122" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -8389,7 +8391,7 @@
         <v>1</v>
       </c>
       <c r="P123" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
@@ -8453,7 +8455,7 @@
         <v>1</v>
       </c>
       <c r="P124" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125">
@@ -8517,7 +8519,7 @@
         <v>1</v>
       </c>
       <c r="P125" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="126">
@@ -9861,7 +9863,7 @@
         <v>1</v>
       </c>
       <c r="P146" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147">
@@ -9925,7 +9927,7 @@
         <v>1</v>
       </c>
       <c r="P147" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -9989,7 +9991,7 @@
         <v>1</v>
       </c>
       <c r="P148" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149">
@@ -10053,7 +10055,7 @@
         <v>1</v>
       </c>
       <c r="P149" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
@@ -10117,7 +10119,7 @@
         <v>1</v>
       </c>
       <c r="P150" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="151">
@@ -10245,7 +10247,7 @@
         <v>1</v>
       </c>
       <c r="P152" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="153">
@@ -10309,7 +10311,7 @@
         <v>1</v>
       </c>
       <c r="P153" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
@@ -10373,7 +10375,7 @@
         <v>1</v>
       </c>
       <c r="P154" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="155">
@@ -10437,7 +10439,7 @@
         <v>1</v>
       </c>
       <c r="P155" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="156">
@@ -10501,7 +10503,7 @@
         <v>1</v>
       </c>
       <c r="P156" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
@@ -10565,7 +10567,7 @@
         <v>1</v>
       </c>
       <c r="P157" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
@@ -10629,7 +10631,7 @@
         <v>1</v>
       </c>
       <c r="P158" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -10693,7 +10695,7 @@
         <v>1</v>
       </c>
       <c r="P159" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160">
@@ -10757,7 +10759,7 @@
         <v>1</v>
       </c>
       <c r="P160" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161">
@@ -10821,7 +10823,7 @@
         <v>1</v>
       </c>
       <c r="P161" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="162">
@@ -10885,7 +10887,7 @@
         <v>1</v>
       </c>
       <c r="P162" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163">
@@ -10949,7 +10951,7 @@
         <v>1</v>
       </c>
       <c r="P163" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="164">
@@ -11013,7 +11015,7 @@
         <v>1</v>
       </c>
       <c r="P164" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="165">
@@ -11205,7 +11207,7 @@
         <v>1</v>
       </c>
       <c r="P167" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
@@ -11269,7 +11271,7 @@
         <v>1</v>
       </c>
       <c r="P168" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="169">
@@ -11333,7 +11335,7 @@
         <v>1</v>
       </c>
       <c r="P169" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
@@ -11397,7 +11399,7 @@
         <v>1</v>
       </c>
       <c r="P170" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="171">
@@ -11589,7 +11591,7 @@
         <v>1</v>
       </c>
       <c r="P173" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="174">
@@ -11653,7 +11655,7 @@
         <v>1</v>
       </c>
       <c r="P174" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="175">
@@ -11717,7 +11719,7 @@
         <v>1</v>
       </c>
       <c r="P175" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">
@@ -11781,7 +11783,7 @@
         <v>1</v>
       </c>
       <c r="P176" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="177">
@@ -11845,7 +11847,7 @@
         <v>1</v>
       </c>
       <c r="P177" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178">
@@ -11909,7 +11911,7 @@
         <v>1</v>
       </c>
       <c r="P178" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="179">
@@ -11973,7 +11975,7 @@
         <v>1</v>
       </c>
       <c r="P179" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="180">
@@ -12101,7 +12103,7 @@
         <v>1</v>
       </c>
       <c r="P181" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182">
@@ -12165,7 +12167,7 @@
         <v>1</v>
       </c>
       <c r="P182" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="183">
@@ -12229,7 +12231,7 @@
         <v>1</v>
       </c>
       <c r="P183" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
@@ -12357,7 +12359,7 @@
         <v>1</v>
       </c>
       <c r="P185" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="186">
@@ -12421,7 +12423,7 @@
         <v>1</v>
       </c>
       <c r="P186" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187">
@@ -12485,7 +12487,7 @@
         <v>1</v>
       </c>
       <c r="P187" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="188">
@@ -12613,7 +12615,7 @@
         <v>1</v>
       </c>
       <c r="P189" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="190">
@@ -12677,7 +12679,7 @@
         <v>1</v>
       </c>
       <c r="P190" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="191">
@@ -12869,7 +12871,7 @@
         <v>1</v>
       </c>
       <c r="P193" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="194">
@@ -12933,7 +12935,7 @@
         <v>1</v>
       </c>
       <c r="P194" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195">
@@ -13061,7 +13063,7 @@
         <v>1</v>
       </c>
       <c r="P196" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="197">
@@ -13509,7 +13511,7 @@
         <v>1</v>
       </c>
       <c r="P203" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="204">
@@ -13573,7 +13575,7 @@
         <v>1</v>
       </c>
       <c r="P204" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="205">
@@ -13637,7 +13639,7 @@
         <v>1</v>
       </c>
       <c r="P205" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="206">
@@ -13765,7 +13767,7 @@
         <v>1</v>
       </c>
       <c r="P207" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="208">
@@ -13829,7 +13831,7 @@
         <v>1</v>
       </c>
       <c r="P208" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="209">
@@ -13893,7 +13895,7 @@
         <v>1</v>
       </c>
       <c r="P209" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="210">
@@ -17605,7 +17607,7 @@
         <v>1</v>
       </c>
       <c r="P267" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="268">
@@ -17669,7 +17671,7 @@
         <v>1</v>
       </c>
       <c r="P268" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="269">
@@ -17733,7 +17735,7 @@
         <v>1</v>
       </c>
       <c r="P269" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="270">
@@ -17797,7 +17799,7 @@
         <v>1</v>
       </c>
       <c r="P270" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
@@ -17861,7 +17863,7 @@
         <v>1</v>
       </c>
       <c r="P271" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="272">
@@ -17925,7 +17927,7 @@
         <v>1</v>
       </c>
       <c r="P272" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="273">
@@ -17989,7 +17991,7 @@
         <v>1</v>
       </c>
       <c r="P273" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274">
@@ -18053,7 +18055,7 @@
         <v>1</v>
       </c>
       <c r="P274" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="275">
@@ -18117,7 +18119,7 @@
         <v>1</v>
       </c>
       <c r="P275" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="276">
@@ -18181,7 +18183,7 @@
         <v>1</v>
       </c>
       <c r="P276" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="277">
@@ -18245,7 +18247,7 @@
         <v>1</v>
       </c>
       <c r="P277" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="278">
@@ -18501,7 +18503,7 @@
         <v>1</v>
       </c>
       <c r="P281" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="282">
@@ -18565,7 +18567,7 @@
         <v>1</v>
       </c>
       <c r="P282" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283">
@@ -18629,7 +18631,7 @@
         <v>1</v>
       </c>
       <c r="P283" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284">
@@ -18693,7 +18695,7 @@
         <v>1</v>
       </c>
       <c r="P284" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="285">
@@ -18757,7 +18759,7 @@
         <v>1</v>
       </c>
       <c r="P285" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="286">
@@ -18821,7 +18823,7 @@
         <v>1</v>
       </c>
       <c r="P286" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="287">
@@ -18885,7 +18887,7 @@
         <v>1</v>
       </c>
       <c r="P287" s="6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="288">
@@ -19348,7 +19350,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
@@ -19369,6 +19371,7 @@
     <col width="12" customWidth="1" min="8" max="8"/>
     <col width="12" customWidth="1" min="9" max="9"/>
     <col width="12" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1" ht="22" customHeight="1">
@@ -19409,7 +19412,7 @@
       </c>
       <c r="H1" s="8" t="inlineStr">
         <is>
-          <t>Location</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="I1" s="8" t="inlineStr">
@@ -19420,6 +19423,11 @@
       <c r="J1" s="8" t="inlineStr">
         <is>
           <t>Time</t>
+        </is>
+      </c>
+      <c r="K1" s="8" t="inlineStr">
+        <is>
+          <t>Validation Group</t>
         </is>
       </c>
     </row>
@@ -25352,7 +25360,70 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J115"/>
+  <autoFilter ref="A1:K115"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" sqref="A1"/>
+      <selection pane="bottomRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" customHeight="1">
+      <c r="A1" s="8" t="inlineStr">
+        <is>
+          <t>Student ID</t>
+        </is>
+      </c>
+      <c r="B1" s="8" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="8" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="D1" s="8" t="inlineStr">
+        <is>
+          <t>Group Before</t>
+        </is>
+      </c>
+      <c r="E1" s="8" t="inlineStr">
+        <is>
+          <t>Group After</t>
+        </is>
+      </c>
+      <c r="F1" s="8" t="inlineStr">
+        <is>
+          <t>Transfer Date</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>